<commit_message>
feat - ajustando filtragem de boletos, e gerando
</commit_message>
<xml_diff>
--- a/src/baseTelefones/Lista Whatsapp RPA.xlsx
+++ b/src/baseTelefones/Lista Whatsapp RPA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="375">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">(35) 99984-8822</t>
   </si>
   <si>
-    <t xml:space="preserve">HEITOR SALAZAR SOARES ( FORMIGA)</t>
+    <t xml:space="preserve">varz</t>
   </si>
   <si>
     <t xml:space="preserve">FRANQUIA 018</t>
@@ -409,7 +409,7 @@
     <t xml:space="preserve">(16) 99786-4768</t>
   </si>
   <si>
-    <t xml:space="preserve">VIWA COMERCIO DE PECAS E SERVICOS AUTOMOTIVOS LTDA( DIVINO</t>
+    <t xml:space="preserve">WIVA COMERCIO DE PEÇAS E SERVIÇOS AUTOMOTIVOS LTDA (DIVINOPOLIS)</t>
   </si>
   <si>
     <t xml:space="preserve">FRANQUIA 020</t>
@@ -709,7 +709,7 @@
     <t xml:space="preserve">(21) 99557-8110</t>
   </si>
   <si>
-    <t xml:space="preserve">JA SERVS AUTOMOTIVOS LTDA ( CAXIAS DO SUL )</t>
+    <t xml:space="preserve">JA SERVICOS AUTOMOTIVOS (CAXIAS DO SUL)</t>
   </si>
   <si>
     <t xml:space="preserve">FRANQUIA 056</t>
@@ -832,7 +832,7 @@
     <t xml:space="preserve">(16) 99728-6091</t>
   </si>
   <si>
-    <t xml:space="preserve">AYOM SERVICOS PECAS E ACESSORIOS LTDA ( DAKAR RIBEIRÃO )</t>
+    <t xml:space="preserve">AYOM SERVICOS PECAS E ACESSORIOS LTDA ( RIBEIRAO PRETO DAKAR </t>
   </si>
   <si>
     <t xml:space="preserve">FRANQUIA 011-01</t>
@@ -856,7 +856,7 @@
     <t xml:space="preserve">(94) 99297-8457</t>
   </si>
   <si>
-    <t xml:space="preserve">FAROL VARZEA PAULISTA COM. ACES. PECAS LTDA ( VARZEA PAULIST</t>
+    <t xml:space="preserve">FAROL VARZEA PAULISTA COMERCIO DE ACESSORIOS E PECAS LTDA ( VARZEA )</t>
   </si>
   <si>
     <t xml:space="preserve">FRANQUIA 046</t>
@@ -958,7 +958,7 @@
     <t xml:space="preserve">(16) 99201-5561</t>
   </si>
   <si>
-    <t xml:space="preserve">SAO JOAQUIM DA BARRA AUTOMOTIVE LTDA ( S.J.BARRA )</t>
+    <t xml:space="preserve">SÃO JOAQUIM DA BARRA AUTOMOTIVE LTDA (S J BARRA)</t>
   </si>
   <si>
     <t xml:space="preserve">FRANQUIA 039</t>
@@ -1006,7 +1006,7 @@
     <t xml:space="preserve">(11) 94304-4427</t>
   </si>
   <si>
-    <t xml:space="preserve">WIVIAN DIAS DURAN ( SÃO JOSE DOS CAMPOS)</t>
+    <t xml:space="preserve">WIVIAN DIAS DURAN (SAO JOSE DOS CAMPOS)</t>
   </si>
   <si>
     <t xml:space="preserve">FRANQUIA 05</t>
@@ -1127,6 +1127,24 @@
   </si>
   <si>
     <t xml:space="preserve">(16) 99162-7434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEONARDO ROCHINSKI COSTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(45) 99808-7365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENZO SETO (MORUMBI) INATIVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(11) 98489-2330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TALITA DIAS DA SILVA (SAO SIMAO) INATIVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(64) 99652-8926</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1155,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1161,7 +1179,7 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -1169,21 +1187,14 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1245,12 +1256,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1258,35 +1269,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1479,42 +1482,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G48" activeCellId="0" sqref="G48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="119.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="8.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="3" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="14.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="2" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1525,19 +1529,19 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1548,19 +1552,19 @@
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1571,19 +1575,19 @@
       <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1594,19 +1598,19 @@
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1617,19 +1621,19 @@
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1640,19 +1644,19 @@
       <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1663,19 +1667,19 @@
       <c r="B8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1686,19 +1690,19 @@
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1709,19 +1713,19 @@
       <c r="B10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1732,19 +1736,19 @@
       <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1755,19 +1759,19 @@
       <c r="B12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1775,19 +1779,19 @@
       <c r="A13" s="1" t="n">
         <v>16388222703</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1798,16 +1802,16 @@
       <c r="B14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1815,22 +1819,22 @@
       <c r="A15" s="1" t="n">
         <v>16335646910</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1841,19 +1845,19 @@
       <c r="B16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1864,19 +1868,19 @@
       <c r="B17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1887,19 +1891,19 @@
       <c r="B18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1910,19 +1914,19 @@
       <c r="B19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1933,19 +1937,19 @@
       <c r="B20" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1956,19 +1960,19 @@
       <c r="B21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1979,16 +1983,16 @@
       <c r="B22" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1999,19 +2003,19 @@
       <c r="B23" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2022,19 +2026,19 @@
       <c r="B24" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2045,16 +2049,16 @@
       <c r="B25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2065,19 +2069,19 @@
       <c r="B26" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="2" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2088,19 +2092,19 @@
       <c r="B27" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2111,19 +2115,19 @@
       <c r="B28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="D28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2134,19 +2138,19 @@
       <c r="B29" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="D29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2157,19 +2161,19 @@
       <c r="B30" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2180,19 +2184,19 @@
       <c r="B31" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="D31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2203,19 +2207,19 @@
       <c r="B32" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2226,19 +2230,19 @@
       <c r="B33" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="D33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2249,19 +2253,19 @@
       <c r="B34" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="D34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2272,19 +2276,19 @@
       <c r="B35" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="D35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2295,16 +2299,16 @@
       <c r="B36" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2315,19 +2319,19 @@
       <c r="B37" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2338,19 +2342,19 @@
       <c r="B38" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2361,16 +2365,16 @@
       <c r="B39" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2381,16 +2385,16 @@
       <c r="B40" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="D40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="2" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2401,13 +2405,13 @@
       <c r="B41" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="3" t="s">
+      <c r="D41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2418,19 +2422,19 @@
       <c r="B42" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="D42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="2" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2441,19 +2445,19 @@
       <c r="B43" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="2" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2464,16 +2468,16 @@
       <c r="B44" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="D44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G44" s="2" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2484,19 +2488,19 @@
       <c r="B45" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="3" t="s">
+      <c r="D45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="2" t="s">
         <v>200</v>
       </c>
     </row>
@@ -2507,19 +2511,19 @@
       <c r="B46" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G46" s="2" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2530,19 +2534,19 @@
       <c r="B47" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="D47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F47" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G47" s="2" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2553,19 +2557,19 @@
       <c r="B48" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="D48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G48" s="2" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2576,19 +2580,19 @@
       <c r="B49" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="3" t="s">
+      <c r="D49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="2" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2599,19 +2603,19 @@
       <c r="B50" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="D50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="G50" s="2" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2622,19 +2626,19 @@
       <c r="B51" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="D51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F51" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="G51" s="2" t="s">
         <v>228</v>
       </c>
     </row>
@@ -2645,19 +2649,19 @@
       <c r="B52" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="D52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="2" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2668,19 +2672,19 @@
       <c r="B53" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="3" t="s">
+      <c r="D53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G53" s="2" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2691,16 +2695,16 @@
       <c r="B54" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="3" t="s">
+      <c r="D54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="G54" s="2" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2711,19 +2715,20 @@
       <c r="B55" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="3" t="s">
+      <c r="D55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G55" s="6"/>
+      <c r="H55" s="2" t="s">
         <v>244</v>
       </c>
     </row>
@@ -2734,16 +2739,16 @@
       <c r="B56" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="D56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G56" s="2" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2751,19 +2756,19 @@
       <c r="A57" s="1" t="n">
         <v>15751788912</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="D57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="2" t="s">
         <v>251</v>
       </c>
     </row>
@@ -2774,16 +2779,16 @@
       <c r="B58" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="3" t="s">
+      <c r="D58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="G58" s="2" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2794,19 +2799,19 @@
       <c r="B59" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="3" t="s">
+      <c r="D59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F59" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="G59" s="2" t="s">
         <v>260</v>
       </c>
     </row>
@@ -2817,19 +2822,19 @@
       <c r="B60" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="D60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G60" s="2" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2840,16 +2845,16 @@
       <c r="B61" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="3" t="s">
+      <c r="D61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="G61" s="2" t="s">
         <v>269</v>
       </c>
     </row>
@@ -2857,22 +2862,22 @@
       <c r="A62" s="1" t="n">
         <v>15698340983</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="3" t="s">
+      <c r="D62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F62" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -2883,19 +2888,19 @@
       <c r="B63" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="3" t="s">
+      <c r="D63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F63" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="G63" s="2" t="s">
         <v>277</v>
       </c>
     </row>
@@ -2906,19 +2911,19 @@
       <c r="B64" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="3" t="s">
+      <c r="D64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F64" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G64" s="2" t="s">
         <v>282</v>
       </c>
     </row>
@@ -2929,19 +2934,19 @@
       <c r="B65" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="3" t="s">
+      <c r="D65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="F65" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G65" s="2" t="s">
         <v>286</v>
       </c>
     </row>
@@ -2952,19 +2957,19 @@
       <c r="B66" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="3" t="s">
+      <c r="D66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="G66" s="2" t="s">
         <v>290</v>
       </c>
     </row>
@@ -2975,19 +2980,19 @@
       <c r="B67" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="3" t="s">
+      <c r="D67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F67" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="G67" s="2" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2998,16 +3003,16 @@
       <c r="B68" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="3" t="s">
+      <c r="D68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="G68" s="2" t="s">
         <v>298</v>
       </c>
     </row>
@@ -3018,19 +3023,19 @@
       <c r="B69" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="3" t="s">
+      <c r="D69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="F69" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="G69" s="3" t="s">
+      <c r="G69" s="2" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3041,16 +3046,16 @@
       <c r="B70" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="D70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="G70" s="2" t="s">
         <v>307</v>
       </c>
     </row>
@@ -3061,16 +3066,16 @@
       <c r="B71" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="3" t="s">
+      <c r="D71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="G71" s="3" t="s">
+      <c r="G71" s="2" t="s">
         <v>311</v>
       </c>
     </row>
@@ -3081,19 +3086,19 @@
       <c r="B72" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="3" t="s">
+      <c r="D72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="F72" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="G72" s="3" t="s">
+      <c r="G72" s="2" t="s">
         <v>315</v>
       </c>
     </row>
@@ -3104,19 +3109,19 @@
       <c r="B73" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="3" t="s">
+      <c r="D73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="F73" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="G73" s="3" t="s">
+      <c r="G73" s="2" t="s">
         <v>319</v>
       </c>
     </row>
@@ -3127,19 +3132,19 @@
       <c r="B74" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="3" t="s">
+      <c r="D74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F74" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="G74" s="2" t="s">
         <v>323</v>
       </c>
     </row>
@@ -3150,19 +3155,19 @@
       <c r="B75" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="3" t="s">
+      <c r="D75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="F75" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="G75" s="2" t="s">
         <v>327</v>
       </c>
     </row>
@@ -3170,22 +3175,22 @@
       <c r="A76" s="1" t="n">
         <v>15689584822</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="3" t="s">
+      <c r="D76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="F76" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="G76" s="3" t="s">
+      <c r="G76" s="2" t="s">
         <v>331</v>
       </c>
     </row>
@@ -3196,19 +3201,19 @@
       <c r="B77" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="3" t="s">
+      <c r="D77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F77" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="G77" s="2" t="s">
         <v>335</v>
       </c>
     </row>
@@ -3219,19 +3224,19 @@
       <c r="B78" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="3" t="s">
+      <c r="D78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="F78" s="3" t="s">
+      <c r="F78" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="G78" s="2" t="s">
         <v>339</v>
       </c>
     </row>
@@ -3242,19 +3247,19 @@
       <c r="B79" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D79" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="3" t="s">
+      <c r="D79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="F79" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="G79" s="2" t="s">
         <v>315</v>
       </c>
     </row>
@@ -3262,13 +3267,13 @@
       <c r="B80" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="10" t="s">
+      <c r="D80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="G80" s="8" t="s">
+      <c r="G80" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -3276,19 +3281,19 @@
       <c r="B81" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="10" t="s">
+      <c r="D81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="F81" s="8" t="s">
+      <c r="F81" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="G81" s="8" t="s">
+      <c r="G81" s="2" t="s">
         <v>349</v>
       </c>
     </row>
@@ -3296,16 +3301,16 @@
       <c r="B82" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="10" t="s">
+      <c r="D82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="G82" s="8" t="s">
+      <c r="G82" s="2" t="s">
         <v>353</v>
       </c>
     </row>
@@ -3313,13 +3318,13 @@
       <c r="B83" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="10" t="s">
+      <c r="D83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="G83" s="8" t="s">
+      <c r="G83" s="2" t="s">
         <v>356</v>
       </c>
     </row>
@@ -3327,16 +3332,16 @@
       <c r="B84" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="10" t="s">
+      <c r="D84" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="G84" s="8" t="s">
+      <c r="G84" s="2" t="s">
         <v>360</v>
       </c>
     </row>
@@ -3344,16 +3349,16 @@
       <c r="B85" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="10" t="s">
+      <c r="D85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="G85" s="8" t="s">
+      <c r="G85" s="2" t="s">
         <v>364</v>
       </c>
     </row>
@@ -3361,8 +3366,7 @@
       <c r="B86" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="F86" s="8"/>
-      <c r="G86" s="8" t="s">
+      <c r="G86" s="2" t="s">
         <v>366</v>
       </c>
     </row>
@@ -3370,8 +3374,32 @@
       <c r="B87" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="G87" s="3" t="s">
+      <c r="G87" s="2" t="s">
         <v>368</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>